<commit_message>
Some recoloring + loot on zone info
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE82A40C-E466-486E-8BC0-A6EC4D7AA4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBCEE04-AC3A-44E0-A69C-6E774155233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
@@ -858,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34C5C6-13B4-428A-8F1D-C41BC0E8B889}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="U55" sqref="U55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,13 +1987,13 @@
         <v>90</v>
       </c>
       <c r="U19">
-        <v>106</v>
+        <v>171</v>
       </c>
       <c r="V19">
-        <v>116</v>
+        <v>210</v>
       </c>
       <c r="W19">
-        <v>125</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
         <v>111</v>
       </c>
       <c r="V21">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="W21">
         <v>122</v>
@@ -2176,13 +2176,13 @@
         <v>145</v>
       </c>
       <c r="U22">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="V22">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="W22">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
@@ -3453,6 +3453,15 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="U46">
+        <v>74</v>
+      </c>
+      <c r="V46">
+        <v>33</v>
+      </c>
+      <c r="W46">
+        <v>117</v>
+      </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -3507,6 +3516,15 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="U47">
+        <v>53</v>
+      </c>
+      <c r="V47">
+        <v>150</v>
+      </c>
+      <c r="W47">
+        <v>83</v>
+      </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
@@ -3561,6 +3579,15 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
+      <c r="U48">
+        <v>22</v>
+      </c>
+      <c r="V48">
+        <v>161</v>
+      </c>
+      <c r="W48">
+        <v>18</v>
+      </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -3678,6 +3705,15 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
+      <c r="U50">
+        <v>9</v>
+      </c>
+      <c r="V50">
+        <v>24</v>
+      </c>
+      <c r="W50">
+        <v>184</v>
+      </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3732,6 +3768,15 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
+      <c r="U51">
+        <v>240</v>
+      </c>
+      <c r="V51">
+        <v>193</v>
+      </c>
+      <c r="W51">
+        <v>65</v>
+      </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -3786,6 +3831,15 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
+      <c r="U52">
+        <v>222</v>
+      </c>
+      <c r="V52">
+        <v>164</v>
+      </c>
+      <c r="W52">
+        <v>78</v>
+      </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
@@ -3903,6 +3957,15 @@
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
+      <c r="U54">
+        <v>168</v>
+      </c>
+      <c r="V54">
+        <v>215</v>
+      </c>
+      <c r="W54">
+        <v>240</v>
+      </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -4095,7 +4158,7 @@
         <v>14</v>
       </c>
       <c r="Q67">
-        <f t="shared" ref="Q67:Q81" si="1">SUM(D67:P67)</f>
+        <f t="shared" ref="Q67:Q71" si="1">SUM(D67:P67)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added a bunch more enemies + Icy Cliffs + GOATMEN :DDD
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBCEE04-AC3A-44E0-A69C-6E774155233B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E0ABF-7D79-4182-B87F-CEB9A95B70F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
@@ -858,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34C5C6-13B4-428A-8F1D-C41BC0E8B889}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="U55" sqref="U55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Upgrade progression system, godot sucks so must use zone name and monster name instead of class_names. :(
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E0ABF-7D79-4182-B87F-CEB9A95B70F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9539A2-7CD1-48D9-BA2B-8E04A9ADF339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
@@ -858,9 +858,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34C5C6-13B4-428A-8F1D-C41BC0E8B889}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I14" sqref="I14"/>
+      <selection pane="topRight" activeCell="R23" sqref="R23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Redo skill equipping / unequipping, progression update
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9539A2-7CD1-48D9-BA2B-8E04A9ADF339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C470F4-3D99-450C-896F-EA34E93B8D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Materials" sheetId="1" r:id="rId1"/>
+    <sheet name="Zones" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$S$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Materials!$A$1:$S$71</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="146">
   <si>
     <t>Oak</t>
   </si>
@@ -356,13 +357,133 @@
   </si>
   <si>
     <t>Troll Hide</t>
+  </si>
+  <si>
+    <t>Easy Forest</t>
+  </si>
+  <si>
+    <t>Medium Forest</t>
+  </si>
+  <si>
+    <t>Hard Forest</t>
+  </si>
+  <si>
+    <t>Easy Desert</t>
+  </si>
+  <si>
+    <t>Medium Desert</t>
+  </si>
+  <si>
+    <t>Hard Desert</t>
+  </si>
+  <si>
+    <t>Ruins</t>
+  </si>
+  <si>
+    <t>Icy Cliffs</t>
+  </si>
+  <si>
+    <t>Ashfallen Forest</t>
+  </si>
+  <si>
+    <t>Pants</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Amulet</t>
+  </si>
+  <si>
+    <t>Easy Beach</t>
+  </si>
+  <si>
+    <t>Medium Beach</t>
+  </si>
+  <si>
+    <t>Hard Beach</t>
+  </si>
+  <si>
+    <t>Easy Town</t>
+  </si>
+  <si>
+    <t>Medium Town</t>
+  </si>
+  <si>
+    <t>Hard Town</t>
+  </si>
+  <si>
+    <t>Bandit Boss</t>
+  </si>
+  <si>
+    <t>Troll Boss</t>
+  </si>
+  <si>
+    <t>Golem Boss</t>
+  </si>
+  <si>
+    <t>Goatman Boss</t>
+  </si>
+  <si>
+    <t>Sword Guard</t>
+  </si>
+  <si>
+    <t>Pommel</t>
+  </si>
+  <si>
+    <t>Secondary Axe Head</t>
+  </si>
+  <si>
+    <t>Shoulders</t>
+  </si>
+  <si>
+    <t>Arms, Shingurads</t>
+  </si>
+  <si>
+    <t>Overpants</t>
+  </si>
+  <si>
+    <t>Boots, Kneepads</t>
+  </si>
+  <si>
+    <t>Visor</t>
+  </si>
+  <si>
+    <t>Neckguard</t>
+  </si>
+  <si>
+    <t>Ornament</t>
+  </si>
+  <si>
+    <t>Calfguards</t>
+  </si>
+  <si>
+    <t>Collars</t>
+  </si>
+  <si>
+    <t>Forearm</t>
+  </si>
+  <si>
+    <t>Crown</t>
+  </si>
+  <si>
+    <t>Beads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -370,8 +491,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -420,6 +562,21 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -430,10 +587,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -443,8 +603,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="3" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -858,9 +1025,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34C5C6-13B4-428A-8F1D-C41BC0E8B889}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R23" sqref="R23"/>
+      <selection pane="topRight" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4398,4 +4565,798 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578E260F-B668-44C6-8E79-CCA2E4813370}">
+  <dimension ref="A1:DQ21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.42578125" style="9"/>
+    <col min="17" max="17" width="10.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="3" style="9" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="121" width="4" style="9" bestFit="1" customWidth="1"/>
+    <col min="122" max="16384" width="4.42578125" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="B1" s="9">
+        <v>5</v>
+      </c>
+      <c r="C1" s="9">
+        <v>10</v>
+      </c>
+      <c r="D1" s="9">
+        <v>15</v>
+      </c>
+      <c r="E1" s="9">
+        <v>20</v>
+      </c>
+      <c r="F1" s="9">
+        <v>25</v>
+      </c>
+      <c r="G1" s="9">
+        <v>30</v>
+      </c>
+      <c r="H1" s="9">
+        <v>35</v>
+      </c>
+      <c r="I1" s="9">
+        <v>40</v>
+      </c>
+      <c r="J1" s="9">
+        <v>45</v>
+      </c>
+      <c r="K1" s="9">
+        <v>50</v>
+      </c>
+      <c r="L1" s="9">
+        <v>55</v>
+      </c>
+      <c r="M1" s="9">
+        <v>60</v>
+      </c>
+      <c r="N1" s="9">
+        <v>65</v>
+      </c>
+      <c r="O1" s="9">
+        <v>70</v>
+      </c>
+      <c r="P1" s="9">
+        <v>75</v>
+      </c>
+      <c r="Q1" s="9">
+        <v>80</v>
+      </c>
+      <c r="R1" s="9">
+        <v>85</v>
+      </c>
+      <c r="S1" s="9">
+        <v>90</v>
+      </c>
+      <c r="T1" s="9">
+        <v>95</v>
+      </c>
+      <c r="U1" s="9">
+        <v>100</v>
+      </c>
+      <c r="V1" s="9">
+        <v>105</v>
+      </c>
+      <c r="W1" s="9">
+        <v>110</v>
+      </c>
+      <c r="X1" s="9">
+        <v>115</v>
+      </c>
+      <c r="Y1" s="9">
+        <v>120</v>
+      </c>
+      <c r="Z1" s="9">
+        <v>125</v>
+      </c>
+      <c r="AA1" s="9">
+        <v>130</v>
+      </c>
+      <c r="AB1" s="9">
+        <v>135</v>
+      </c>
+      <c r="AC1" s="9">
+        <v>140</v>
+      </c>
+      <c r="AD1" s="9">
+        <v>145</v>
+      </c>
+      <c r="AE1" s="9">
+        <v>150</v>
+      </c>
+      <c r="AF1" s="9">
+        <v>155</v>
+      </c>
+      <c r="AG1" s="9">
+        <v>160</v>
+      </c>
+      <c r="AH1" s="9">
+        <v>165</v>
+      </c>
+      <c r="AI1" s="9">
+        <v>170</v>
+      </c>
+      <c r="AJ1" s="9">
+        <v>175</v>
+      </c>
+      <c r="AK1" s="9">
+        <v>180</v>
+      </c>
+      <c r="AL1" s="9">
+        <v>185</v>
+      </c>
+      <c r="AM1" s="9">
+        <v>190</v>
+      </c>
+      <c r="AN1" s="9">
+        <v>195</v>
+      </c>
+      <c r="AO1" s="9">
+        <v>200</v>
+      </c>
+      <c r="AP1" s="9">
+        <v>205</v>
+      </c>
+      <c r="AQ1" s="9">
+        <v>210</v>
+      </c>
+      <c r="AR1" s="9">
+        <v>215</v>
+      </c>
+      <c r="AS1" s="9">
+        <v>220</v>
+      </c>
+      <c r="AT1" s="9">
+        <v>225</v>
+      </c>
+      <c r="AU1" s="9">
+        <v>230</v>
+      </c>
+      <c r="AV1" s="9">
+        <v>235</v>
+      </c>
+      <c r="AW1" s="9">
+        <v>240</v>
+      </c>
+      <c r="AX1" s="9">
+        <v>245</v>
+      </c>
+      <c r="AY1" s="9">
+        <v>250</v>
+      </c>
+      <c r="AZ1" s="9">
+        <v>255</v>
+      </c>
+      <c r="BA1" s="9">
+        <v>260</v>
+      </c>
+      <c r="BB1" s="9">
+        <v>265</v>
+      </c>
+      <c r="BC1" s="9">
+        <v>270</v>
+      </c>
+      <c r="BD1" s="9">
+        <v>275</v>
+      </c>
+      <c r="BE1" s="9">
+        <v>280</v>
+      </c>
+      <c r="BF1" s="9">
+        <v>285</v>
+      </c>
+      <c r="BG1" s="9">
+        <v>290</v>
+      </c>
+      <c r="BH1" s="9">
+        <v>295</v>
+      </c>
+      <c r="BI1" s="9">
+        <v>300</v>
+      </c>
+      <c r="BJ1" s="9">
+        <v>305</v>
+      </c>
+      <c r="BK1" s="9">
+        <v>310</v>
+      </c>
+      <c r="BL1" s="9">
+        <v>315</v>
+      </c>
+      <c r="BM1" s="9">
+        <v>320</v>
+      </c>
+      <c r="BN1" s="9">
+        <v>325</v>
+      </c>
+      <c r="BO1" s="9">
+        <v>330</v>
+      </c>
+      <c r="BP1" s="9">
+        <v>335</v>
+      </c>
+      <c r="BQ1" s="9">
+        <v>340</v>
+      </c>
+      <c r="BR1" s="9">
+        <v>345</v>
+      </c>
+      <c r="BS1" s="9">
+        <v>350</v>
+      </c>
+      <c r="BT1" s="9">
+        <v>355</v>
+      </c>
+      <c r="BU1" s="9">
+        <v>360</v>
+      </c>
+      <c r="BV1" s="9">
+        <v>365</v>
+      </c>
+      <c r="BW1" s="9">
+        <v>370</v>
+      </c>
+      <c r="BX1" s="9">
+        <v>375</v>
+      </c>
+      <c r="BY1" s="9">
+        <v>380</v>
+      </c>
+      <c r="BZ1" s="9">
+        <v>385</v>
+      </c>
+      <c r="CA1" s="9">
+        <v>390</v>
+      </c>
+      <c r="CB1" s="9">
+        <v>395</v>
+      </c>
+      <c r="CC1" s="9">
+        <v>400</v>
+      </c>
+      <c r="CD1" s="9">
+        <v>405</v>
+      </c>
+      <c r="CE1" s="9">
+        <v>410</v>
+      </c>
+      <c r="CF1" s="9">
+        <v>415</v>
+      </c>
+      <c r="CG1" s="9">
+        <v>420</v>
+      </c>
+      <c r="CH1" s="9">
+        <v>425</v>
+      </c>
+      <c r="CI1" s="9">
+        <v>430</v>
+      </c>
+      <c r="CJ1" s="9">
+        <v>435</v>
+      </c>
+      <c r="CK1" s="9">
+        <v>440</v>
+      </c>
+      <c r="CL1" s="9">
+        <v>445</v>
+      </c>
+      <c r="CM1" s="9">
+        <v>450</v>
+      </c>
+      <c r="CN1" s="9">
+        <v>455</v>
+      </c>
+      <c r="CO1" s="9">
+        <v>460</v>
+      </c>
+      <c r="CP1" s="9">
+        <v>465</v>
+      </c>
+      <c r="CQ1" s="9">
+        <v>470</v>
+      </c>
+      <c r="CR1" s="9">
+        <v>475</v>
+      </c>
+      <c r="CS1" s="9">
+        <v>480</v>
+      </c>
+      <c r="CT1" s="9">
+        <v>485</v>
+      </c>
+      <c r="CU1" s="9">
+        <v>490</v>
+      </c>
+      <c r="CV1" s="9">
+        <v>495</v>
+      </c>
+      <c r="CW1" s="9">
+        <v>500</v>
+      </c>
+      <c r="CX1" s="9">
+        <v>505</v>
+      </c>
+      <c r="CY1" s="9">
+        <v>510</v>
+      </c>
+      <c r="CZ1" s="9">
+        <v>515</v>
+      </c>
+      <c r="DA1" s="9">
+        <v>520</v>
+      </c>
+      <c r="DB1" s="9">
+        <v>525</v>
+      </c>
+      <c r="DC1" s="9">
+        <v>530</v>
+      </c>
+      <c r="DD1" s="9">
+        <v>535</v>
+      </c>
+      <c r="DE1" s="9">
+        <v>540</v>
+      </c>
+      <c r="DF1" s="9">
+        <v>545</v>
+      </c>
+      <c r="DG1" s="9">
+        <v>550</v>
+      </c>
+      <c r="DH1" s="9">
+        <v>555</v>
+      </c>
+      <c r="DI1" s="9">
+        <v>560</v>
+      </c>
+      <c r="DJ1" s="9">
+        <v>565</v>
+      </c>
+      <c r="DK1" s="9">
+        <v>570</v>
+      </c>
+      <c r="DL1" s="9">
+        <v>575</v>
+      </c>
+      <c r="DM1" s="9">
+        <v>580</v>
+      </c>
+      <c r="DN1" s="9">
+        <v>585</v>
+      </c>
+      <c r="DO1" s="9">
+        <v>590</v>
+      </c>
+      <c r="DP1" s="9">
+        <v>595</v>
+      </c>
+      <c r="DQ1" s="9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="2" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="4" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="V4" s="12"/>
+      <c r="W4" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="L6" s="12"/>
+      <c r="M6" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" s="12"/>
+      <c r="Y8" s="12"/>
+      <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+    </row>
+    <row r="9" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
+      <c r="Y9" s="12"/>
+      <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="12"/>
+      <c r="AJ9" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK9" s="12"/>
+      <c r="AL9" s="12"/>
+      <c r="AM9" s="12"/>
+      <c r="AN9" s="12"/>
+      <c r="AO9" s="12"/>
+    </row>
+    <row r="10" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
+      <c r="AK10" s="12"/>
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="12"/>
+      <c r="AT10" s="12"/>
+      <c r="AU10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="AW10" s="12"/>
+      <c r="AX10" s="12"/>
+      <c r="AY10" s="12"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="12"/>
+      <c r="BB10" s="12"/>
+      <c r="BC10" s="12"/>
+      <c r="BD10" s="12"/>
+      <c r="BE10" s="12"/>
+      <c r="BF10" s="12"/>
+      <c r="BG10" s="12"/>
+      <c r="BH10" s="12"/>
+      <c r="BI10" s="12"/>
+    </row>
+    <row r="11" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="12"/>
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12"/>
+      <c r="AN11" s="12"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="12"/>
+      <c r="AQ11" s="12"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="12"/>
+      <c r="AT11" s="12"/>
+    </row>
+    <row r="12" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="AU12" s="12"/>
+      <c r="AV12" s="12"/>
+      <c r="AW12" s="12"/>
+      <c r="AX12" s="12"/>
+      <c r="AY12" s="12"/>
+      <c r="AZ12" s="12"/>
+      <c r="BA12" s="12"/>
+      <c r="BB12" s="12"/>
+      <c r="BC12" s="12"/>
+      <c r="BD12" s="12"/>
+      <c r="BE12" s="12"/>
+      <c r="BF12" s="12"/>
+      <c r="BG12" s="12"/>
+      <c r="BH12" s="12"/>
+      <c r="BI12" s="12"/>
+    </row>
+    <row r="13" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="BJ13" s="12"/>
+      <c r="BK13" s="12"/>
+      <c r="BL13" s="12"/>
+      <c r="BM13" s="12"/>
+      <c r="BN13" s="12"/>
+      <c r="BO13" s="12"/>
+      <c r="BP13" s="12"/>
+      <c r="BQ13" s="12"/>
+      <c r="BR13" s="12"/>
+      <c r="BS13" s="12"/>
+      <c r="BT13" s="12"/>
+      <c r="BU13" s="12"/>
+      <c r="BV13" s="12"/>
+      <c r="BW13" s="12"/>
+      <c r="BX13" s="12"/>
+      <c r="BY13" s="12"/>
+      <c r="BZ13" s="12"/>
+      <c r="CA13" s="12"/>
+      <c r="CB13" s="12"/>
+      <c r="CC13" s="12"/>
+    </row>
+    <row r="14" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO14" s="12"/>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="12"/>
+      <c r="AT14" s="12"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="12"/>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="12"/>
+      <c r="AZ14" s="12"/>
+      <c r="BA14" s="12"/>
+      <c r="BB14" s="12"/>
+      <c r="BC14" s="12"/>
+      <c r="BD14" s="12"/>
+      <c r="BE14" s="12"/>
+      <c r="BF14" s="12"/>
+      <c r="BG14" s="12"/>
+      <c r="BH14" s="12"/>
+      <c r="BI14" s="12"/>
+    </row>
+    <row r="15" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="BJ15" s="12"/>
+      <c r="BK15" s="12"/>
+      <c r="BL15" s="12"/>
+      <c r="BM15" s="12"/>
+      <c r="BN15" s="12"/>
+      <c r="BO15" s="12"/>
+      <c r="BP15" s="12"/>
+      <c r="BQ15" s="12"/>
+      <c r="BR15" s="12"/>
+      <c r="BS15" s="12"/>
+      <c r="BT15" s="12"/>
+      <c r="BU15" s="12"/>
+      <c r="BV15" s="12"/>
+      <c r="BW15" s="12"/>
+      <c r="BX15" s="12"/>
+      <c r="BY15" s="12"/>
+      <c r="BZ15" s="12"/>
+      <c r="CA15" s="12"/>
+      <c r="CB15" s="12"/>
+      <c r="CC15" s="12"/>
+      <c r="CD15" s="12"/>
+      <c r="CE15" s="12"/>
+      <c r="CF15" s="12"/>
+      <c r="CG15" s="12"/>
+      <c r="CH15" s="12"/>
+    </row>
+    <row r="16" spans="1:121" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="CI16" s="12"/>
+      <c r="CJ16" s="12"/>
+      <c r="CK16" s="12"/>
+      <c r="CL16" s="12"/>
+      <c r="CM16" s="12"/>
+      <c r="CN16" s="12"/>
+      <c r="CO16" s="12"/>
+      <c r="CP16" s="12"/>
+      <c r="CQ16" s="12"/>
+      <c r="CR16" s="12"/>
+      <c r="CS16" s="12"/>
+      <c r="CT16" s="12"/>
+      <c r="CU16" s="12"/>
+      <c r="CV16" s="12"/>
+      <c r="CW16" s="12"/>
+      <c r="CX16" s="12"/>
+      <c r="CY16" s="12"/>
+      <c r="CZ16" s="12"/>
+      <c r="DA16" s="12"/>
+      <c r="DB16" s="12"/>
+      <c r="DC16" s="12"/>
+      <c r="DD16" s="12"/>
+      <c r="DE16" s="12"/>
+      <c r="DF16" s="12"/>
+      <c r="DG16" s="12"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Material distribution rebalancing + quests work offline now
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C470F4-3D99-450C-896F-EA34E93B8D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F24A1F-B3F8-42AB-96CB-39979CDEF09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -1026,8 +1026,8 @@
   <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,11 +2021,11 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="Q17">
         <f t="shared" si="0"/>
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="U17">
         <v>168</v>
@@ -2138,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N19">
         <v>15</v>
@@ -2147,11 +2147,11 @@
         <v>0</v>
       </c>
       <c r="P19">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="Q19">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="U19">
         <v>171</v>
@@ -2369,7 +2369,7 @@
         <v>5</v>
       </c>
       <c r="F23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G23">
         <v>20</v>
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="J23">
         <v>20</v>
@@ -2387,10 +2387,10 @@
         <v>0</v>
       </c>
       <c r="L23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M23">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="N23">
         <v>20</v>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="P23">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="Q23">
         <f t="shared" si="0"/>
@@ -4572,7 +4572,7 @@
   <dimension ref="A1:DQ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5085,7 +5085,7 @@
       <c r="A8" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8"/>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
@@ -5116,11 +5116,11 @@
       <c r="A9" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="V9" s="12"/>
-      <c r="W9" s="12"/>
-      <c r="X9" s="12"/>
-      <c r="Y9" s="12"/>
-      <c r="Z9" s="12"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
       <c r="AC9" s="12"/>

</xml_diff>

<commit_message>
Rebalanced costs + waaaay better ui for part making
</commit_message>
<xml_diff>
--- a/MaterialImporter/Materials.xlsx
+++ b/MaterialImporter/Materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marko\Documents\Idle Dungeon Runner\MaterialImporter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DF807E-6380-4F5F-9CF1-A56C0D2A4962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBE1F46-C293-4751-BCBC-54B7BB4E06E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{31B0E43A-1B63-48EF-9D20-16AE13CC56BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -1025,7 +1025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA34C5C6-13B4-428A-8F1D-C41BC0E8B889}">
   <dimension ref="A1:W71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G32" sqref="G32"/>
     </sheetView>
@@ -4571,8 +4571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578E260F-B668-44C6-8E79-CCA2E4813370}">
   <dimension ref="A1:DQ21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>